<commit_message>
Make students complete DQ 1 first!
</commit_message>
<xml_diff>
--- a/144F20/Topic 6/Topic 6 DQ 1 and 2.xlsx
+++ b/144F20/Topic 6/Topic 6 DQ 1 and 2.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gcumail-my.sharepoint.com/personal/richard_ketchersid_gcu_edu/Documents/Course Materials/git/Teaching/144F20/Topic 6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{A4867632-43AB-4763-8819-0561CF9679FB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{1EB18961-7277-4991-B4D1-A40B51C69814}"/>
+  <xr:revisionPtr revIDLastSave="75" documentId="8_{A4867632-43AB-4763-8819-0561CF9679FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{48C2B13F-3069-418D-90E6-F118965F33BC}"/>
   <bookViews>
-    <workbookView xWindow="7050" yWindow="1305" windowWidth="20100" windowHeight="10890" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2220" yWindow="2115" windowWidth="20070" windowHeight="12900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hand DQ1" sheetId="1" r:id="rId1"/>
     <sheet name="Formulas DQ2" sheetId="6" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="7" state="hidden" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="8" state="hidden" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="7" state="hidden" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="191029" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -32,6 +33,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -315,9 +338,6 @@
     <t>Create a histogram using the Excel (clustered) column chart (2D or 3D).</t>
   </si>
   <si>
-    <t>Now repeat the first part, but using Excel formulas and charts.</t>
-  </si>
-  <si>
     <t>Click on links for video instruction.</t>
   </si>
   <si>
@@ -577,6 +597,9 @@
   </si>
   <si>
     <t>Your Name</t>
+  </si>
+  <si>
+    <t>Repeat using formulas. You MUST complete "Hand DQ 1" first!</t>
   </si>
 </sst>
 </file>
@@ -1111,102 +1134,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1242,6 +1169,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1250,6 +1186,93 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1299,7 +1322,64 @@
     <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="8">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color rgb="FF339933"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="0" tint="-0.24994659260841701"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="0" tint="-0.34998626667073579"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color theme="0" tint="-0.24994659260841701"/>
@@ -1322,6 +1402,11 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF339933"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1334,6 +1419,102 @@
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>352425</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="2796791" cy="609013"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{523B523B-74AB-4342-84BC-7508BA77C4DE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7962900" y="3133725"/>
+          <a:ext cx="2796791" cy="609013"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:solidFill>
+            <a:schemeClr val="accent6">
+              <a:lumMod val="75000"/>
+            </a:schemeClr>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>The frequency numbers must be all correct</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>and </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1">
+              <a:solidFill>
+                <a:srgbClr val="339933"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>green</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t> before "Formulas DQ 2" will show</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>correctly.</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -1413,6 +1594,61 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="184731" cy="264560"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3C518383-B089-426F-8177-65A50E98F95E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7896225" y="266700"/>
+          <a:ext cx="184731" cy="264560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1682,7 +1918,7 @@
   <dimension ref="A1:K56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1690,41 +1926,41 @@
     <col min="1" max="1" width="17" customWidth="1"/>
     <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="8" max="8" width="18" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="21" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75" thickBot="1">
-      <c r="D1" s="45" t="s">
-        <v>111</v>
-      </c>
-      <c r="E1" s="46"/>
-      <c r="F1" s="46"/>
-      <c r="G1" s="46"/>
-      <c r="H1" s="47"/>
+      <c r="D1" s="65" t="s">
+        <v>110</v>
+      </c>
+      <c r="E1" s="66"/>
+      <c r="F1" s="66"/>
+      <c r="G1" s="66"/>
+      <c r="H1" s="67"/>
     </row>
     <row r="2" spans="1:11" ht="18" thickBot="1">
       <c r="A2" s="42" t="s">
-        <v>110</v>
-      </c>
-      <c r="B2" s="43" t="s">
-        <v>169</v>
-      </c>
-      <c r="C2" s="44"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="50"/>
+        <v>109</v>
+      </c>
+      <c r="B2" s="63" t="s">
+        <v>168</v>
+      </c>
+      <c r="C2" s="64"/>
+      <c r="D2" s="68"/>
+      <c r="E2" s="69"/>
+      <c r="F2" s="69"/>
+      <c r="G2" s="69"/>
+      <c r="H2" s="70"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" thickBot="1">
-      <c r="D3" s="51"/>
-      <c r="E3" s="52"/>
-      <c r="F3" s="52"/>
-      <c r="G3" s="52"/>
-      <c r="H3" s="53"/>
+      <c r="D3" s="71"/>
+      <c r="E3" s="72"/>
+      <c r="F3" s="72"/>
+      <c r="G3" s="72"/>
+      <c r="H3" s="73"/>
     </row>
     <row r="5" spans="1:11" ht="15.75" thickBot="1"/>
     <row r="6" spans="1:11" ht="15.75">
@@ -1734,17 +1970,17 @@
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="77" t="s">
+      <c r="D6" s="45" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="78"/>
-      <c r="F6" s="78"/>
-      <c r="G6" s="78"/>
-      <c r="H6" s="79"/>
-      <c r="J6" s="75" t="s">
+      <c r="E6" s="46"/>
+      <c r="F6" s="46"/>
+      <c r="G6" s="46"/>
+      <c r="H6" s="47"/>
+      <c r="J6" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="76"/>
+      <c r="K6" s="44"/>
     </row>
     <row r="7" spans="1:11" ht="14.45" customHeight="1" thickBot="1">
       <c r="A7" s="5" t="s">
@@ -1754,11 +1990,11 @@
         <f ca="1">Sheet1!K20</f>
         <v>112</v>
       </c>
-      <c r="D7" s="80"/>
-      <c r="E7" s="81"/>
-      <c r="F7" s="81"/>
-      <c r="G7" s="81"/>
-      <c r="H7" s="82"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="49"/>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="50"/>
       <c r="J7" s="7" t="s">
         <v>53</v>
       </c>
@@ -1797,13 +2033,13 @@
       <c r="C9" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="83" t="s">
+      <c r="D9" s="51" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="84"/>
-      <c r="F9" s="85"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="53"/>
       <c r="G9" s="39" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H9" s="15"/>
       <c r="J9" s="11" t="s">
@@ -1824,14 +2060,14 @@
       <c r="C10" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="83" t="s">
+      <c r="D10" s="51" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="84"/>
-      <c r="F10" s="85"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="53"/>
       <c r="G10" s="18"/>
       <c r="H10" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J10" s="12" t="s">
         <v>59</v>
@@ -1849,13 +2085,13 @@
         <v>142</v>
       </c>
       <c r="C11" s="16"/>
-      <c r="D11" s="60" t="s">
-        <v>84</v>
-      </c>
-      <c r="E11" s="61"/>
-      <c r="F11" s="61"/>
-      <c r="G11" s="61"/>
-      <c r="H11" s="62"/>
+      <c r="D11" s="74" t="s">
+        <v>83</v>
+      </c>
+      <c r="E11" s="75"/>
+      <c r="F11" s="75"/>
+      <c r="G11" s="75"/>
+      <c r="H11" s="76"/>
       <c r="J11" s="13" t="s">
         <v>61</v>
       </c>
@@ -1871,11 +2107,11 @@
         <f ca="1">Sheet1!K25</f>
         <v>118</v>
       </c>
-      <c r="D12" s="63"/>
-      <c r="E12" s="64"/>
-      <c r="F12" s="64"/>
-      <c r="G12" s="64"/>
-      <c r="H12" s="65"/>
+      <c r="D12" s="77"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
+      <c r="H12" s="79"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="5" t="s">
@@ -1885,11 +2121,11 @@
         <f ca="1">Sheet1!K26</f>
         <v>106</v>
       </c>
-      <c r="D13" s="63"/>
-      <c r="E13" s="64"/>
-      <c r="F13" s="64"/>
-      <c r="G13" s="64"/>
-      <c r="H13" s="65"/>
+      <c r="D13" s="77"/>
+      <c r="E13" s="78"/>
+      <c r="F13" s="78"/>
+      <c r="G13" s="78"/>
+      <c r="H13" s="79"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1">
       <c r="A14" s="5" t="s">
@@ -1899,11 +2135,11 @@
         <f ca="1">Sheet1!K27</f>
         <v>110</v>
       </c>
-      <c r="D14" s="66"/>
-      <c r="E14" s="67"/>
-      <c r="F14" s="67"/>
-      <c r="G14" s="67"/>
-      <c r="H14" s="68"/>
+      <c r="D14" s="80"/>
+      <c r="E14" s="81"/>
+      <c r="F14" s="81"/>
+      <c r="G14" s="81"/>
+      <c r="H14" s="82"/>
     </row>
     <row r="15" spans="1:11" ht="15.75" thickBot="1">
       <c r="A15" s="5" t="s">
@@ -1916,14 +2152,14 @@
       <c r="C15" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="69" t="s">
+      <c r="D15" s="83" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="70"/>
-      <c r="F15" s="71"/>
+      <c r="E15" s="84"/>
+      <c r="F15" s="85"/>
       <c r="G15" s="18"/>
       <c r="H15" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1">
@@ -1937,13 +2173,13 @@
       <c r="C16" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="72" t="s">
+      <c r="D16" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="73"/>
-      <c r="F16" s="74"/>
+      <c r="E16" s="87"/>
+      <c r="F16" s="88"/>
       <c r="G16" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="H16" s="2"/>
     </row>
@@ -2093,11 +2329,11 @@
         <f ca="1">Sheet1!K38</f>
         <v>111</v>
       </c>
-      <c r="D25" s="86"/>
-      <c r="E25" s="87"/>
-      <c r="F25" s="87"/>
-      <c r="G25" s="87"/>
-      <c r="H25" s="88"/>
+      <c r="D25" s="57"/>
+      <c r="E25" s="58"/>
+      <c r="F25" s="58"/>
+      <c r="G25" s="58"/>
+      <c r="H25" s="59"/>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="5" t="s">
@@ -2107,11 +2343,11 @@
         <f ca="1">Sheet1!K39</f>
         <v>109</v>
       </c>
-      <c r="D26" s="86"/>
-      <c r="E26" s="87"/>
-      <c r="F26" s="87"/>
-      <c r="G26" s="87"/>
-      <c r="H26" s="88"/>
+      <c r="D26" s="57"/>
+      <c r="E26" s="58"/>
+      <c r="F26" s="58"/>
+      <c r="G26" s="58"/>
+      <c r="H26" s="59"/>
     </row>
     <row r="27" spans="1:11" ht="15.75" thickBot="1">
       <c r="A27" s="5" t="s">
@@ -2121,11 +2357,11 @@
         <f ca="1">Sheet1!K40</f>
         <v>104</v>
       </c>
-      <c r="D27" s="57"/>
-      <c r="E27" s="58"/>
-      <c r="F27" s="58"/>
-      <c r="G27" s="58"/>
-      <c r="H27" s="59"/>
+      <c r="D27" s="60"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="G27" s="61"/>
+      <c r="H27" s="62"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="5" t="s">
@@ -2146,7 +2382,7 @@
       <c r="G28" s="55"/>
       <c r="H28" s="56"/>
       <c r="I28" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="29" spans="1:11" ht="15.75" thickBot="1">
@@ -2157,11 +2393,11 @@
         <f ca="1">Sheet1!K42</f>
         <v>114</v>
       </c>
-      <c r="D29" s="57"/>
-      <c r="E29" s="58"/>
-      <c r="F29" s="58"/>
-      <c r="G29" s="58"/>
-      <c r="H29" s="59"/>
+      <c r="D29" s="60"/>
+      <c r="E29" s="61"/>
+      <c r="F29" s="61"/>
+      <c r="G29" s="61"/>
+      <c r="H29" s="62"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="5" t="s">
@@ -2605,20 +2841,20 @@
     <sortCondition ref="A7:A57"/>
   </sortState>
   <mergeCells count="11">
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="D6:H7"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D24:H27"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D1:H3"/>
     <mergeCell ref="D28:H29"/>
     <mergeCell ref="D11:H14"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D16:F16"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="D6:H7"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D24:H27"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:K56">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="1" priority="2">
       <formula>$B$2="Your Name"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2631,6 +2867,26 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId6"/>
+  <drawing r:id="rId7"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{E6DB032A-3596-4684-BCEA-B31F9EBB35F6}">
+            <xm:f>G18=Sheet2!$A1</xm:f>
+            <x14:dxf>
+              <font>
+                <b/>
+                <i val="0"/>
+                <color rgb="FF339933"/>
+              </font>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>G18:G23</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -2639,7 +2895,7 @@
   <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B51"/>
+      <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2649,8 +2905,8 @@
     <col min="4" max="7" width="13.7109375" customWidth="1"/>
     <col min="8" max="8" width="16.42578125" customWidth="1"/>
     <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16" customWidth="1"/>
+    <col min="11" max="11" width="21.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="15.75">
@@ -2661,16 +2917,16 @@
         <v>1</v>
       </c>
       <c r="D1" s="96" t="s">
-        <v>82</v>
+        <v>169</v>
       </c>
       <c r="E1" s="97"/>
       <c r="F1" s="97"/>
       <c r="G1" s="97"/>
       <c r="H1" s="98"/>
-      <c r="J1" s="75" t="s">
+      <c r="J1" s="43" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="76"/>
+      <c r="K1" s="44"/>
     </row>
     <row r="2" spans="1:11" ht="14.45" customHeight="1" thickBot="1">
       <c r="A2" s="5" t="s">
@@ -2730,7 +2986,7 @@
       <c r="F4" s="34"/>
       <c r="G4" s="35"/>
       <c r="H4" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="J4" s="11" t="s">
         <v>57</v>
@@ -2770,11 +3026,11 @@
         <f ca="1">Sheet1!K24</f>
         <v>142</v>
       </c>
-      <c r="D6" s="86"/>
-      <c r="E6" s="87"/>
-      <c r="F6" s="87"/>
-      <c r="G6" s="87"/>
-      <c r="H6" s="88"/>
+      <c r="D6" s="57"/>
+      <c r="E6" s="58"/>
+      <c r="F6" s="58"/>
+      <c r="G6" s="58"/>
+      <c r="H6" s="59"/>
       <c r="J6" s="13" t="s">
         <v>61</v>
       </c>
@@ -2790,11 +3046,11 @@
         <f ca="1">Sheet1!K25</f>
         <v>118</v>
       </c>
-      <c r="D7" s="86"/>
-      <c r="E7" s="87"/>
-      <c r="F7" s="87"/>
-      <c r="G7" s="87"/>
-      <c r="H7" s="88"/>
+      <c r="D7" s="57"/>
+      <c r="E7" s="58"/>
+      <c r="F7" s="58"/>
+      <c r="G7" s="58"/>
+      <c r="H7" s="59"/>
     </row>
     <row r="8" spans="1:11" ht="15.75" thickBot="1">
       <c r="A8" s="5" t="s">
@@ -2804,11 +3060,11 @@
         <f ca="1">Sheet1!K26</f>
         <v>106</v>
       </c>
-      <c r="D8" s="57"/>
-      <c r="E8" s="58"/>
-      <c r="F8" s="58"/>
-      <c r="G8" s="58"/>
-      <c r="H8" s="59"/>
+      <c r="D8" s="60"/>
+      <c r="E8" s="61"/>
+      <c r="F8" s="61"/>
+      <c r="G8" s="61"/>
+      <c r="H8" s="62"/>
     </row>
     <row r="9" spans="1:11" ht="15.75" thickBot="1">
       <c r="A9" s="5" t="s">
@@ -2821,14 +3077,14 @@
       <c r="C9" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="69" t="s">
+      <c r="D9" s="83" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="70"/>
-      <c r="F9" s="71"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="85"/>
       <c r="G9" s="35"/>
       <c r="H9" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" thickBot="1">
@@ -2842,16 +3098,16 @@
       <c r="C10" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="72" t="s">
+      <c r="D10" s="86" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="73"/>
-      <c r="F10" s="74"/>
+      <c r="E10" s="87"/>
+      <c r="F10" s="88"/>
       <c r="G10" s="40" t="s">
+        <v>84</v>
+      </c>
+      <c r="H10" s="102" t="s">
         <v>85</v>
-      </c>
-      <c r="H10" s="102" t="s">
-        <v>86</v>
       </c>
       <c r="I10" s="102"/>
       <c r="J10" s="102"/>
@@ -2880,7 +3136,7 @@
         <v>77</v>
       </c>
       <c r="I11" s="95" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J11" s="95"/>
       <c r="K11" s="95"/>
@@ -3006,11 +3262,11 @@
         <f ca="1">Sheet1!K37</f>
         <v>114</v>
       </c>
-      <c r="D19" s="86"/>
-      <c r="E19" s="87"/>
-      <c r="F19" s="87"/>
-      <c r="G19" s="87"/>
-      <c r="H19" s="88"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="58"/>
+      <c r="F19" s="58"/>
+      <c r="G19" s="58"/>
+      <c r="H19" s="59"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="5" t="s">
@@ -3020,11 +3276,11 @@
         <f ca="1">Sheet1!K38</f>
         <v>111</v>
       </c>
-      <c r="D20" s="86"/>
-      <c r="E20" s="87"/>
-      <c r="F20" s="87"/>
-      <c r="G20" s="87"/>
-      <c r="H20" s="88"/>
+      <c r="D20" s="57"/>
+      <c r="E20" s="58"/>
+      <c r="F20" s="58"/>
+      <c r="G20" s="58"/>
+      <c r="H20" s="59"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" thickBot="1">
       <c r="A21" s="5" t="s">
@@ -3034,11 +3290,11 @@
         <f ca="1">Sheet1!K39</f>
         <v>109</v>
       </c>
-      <c r="D21" s="57"/>
-      <c r="E21" s="58"/>
-      <c r="F21" s="58"/>
-      <c r="G21" s="58"/>
-      <c r="H21" s="59"/>
+      <c r="D21" s="60"/>
+      <c r="E21" s="61"/>
+      <c r="F21" s="61"/>
+      <c r="G21" s="61"/>
+      <c r="H21" s="62"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="5" t="s">
@@ -3059,7 +3315,7 @@
       <c r="G22" s="90"/>
       <c r="H22" s="91"/>
       <c r="I22" s="40" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" thickBot="1">
@@ -3369,7 +3625,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="expression" priority="1" id="{DFFB5F44-41EC-4BE2-B855-809370786DC3}">
+          <x14:cfRule type="expression" priority="2" id="{DFFB5F44-41EC-4BE2-B855-809370786DC3}">
             <xm:f>'Hand DQ1'!$B$2="Your Name"</xm:f>
             <x14:dxf>
               <font>
@@ -3384,6 +3640,22 @@
           </x14:cfRule>
           <xm:sqref>A1:XFD1048576</xm:sqref>
         </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="expression" priority="1" id="{4321C13B-9D9E-4142-9612-9189A609C798}">
+            <xm:f>Sheet2!$D$1=FALSE</xm:f>
+            <x14:dxf>
+              <font>
+                <color theme="0" tint="-0.24994659260841701"/>
+              </font>
+              <fill>
+                <patternFill>
+                  <bgColor theme="0" tint="-0.34998626667073579"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>A3:XFD1048576</xm:sqref>
+        </x14:conditionalFormatting>
       </x14:conditionalFormattings>
     </ext>
   </extLst>
@@ -3391,6 +3663,64 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3206DDE0-65A2-4525-995F-49F65095EBC3}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" cm="1">
+        <f t="array" aca="1" ref="A1:A2" ca="1">FREQUENCY('Hand DQ1'!B7:B56,'Hand DQ1'!F18:F22)</f>
+        <v>0</v>
+      </c>
+      <c r="B1" cm="1">
+        <f t="array" ref="B1:B6">'Hand DQ1'!G18:G23</f>
+        <v>0</v>
+      </c>
+      <c r="D1" t="e" cm="1">
+        <f t="array" aca="1" ref="D1" ca="1">AND(_xlfn.ANCHORARRAY(A1)=_xlfn.ANCHORARRAY(B1))</f>
+        <v>#N/A</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2">
+        <f ca="1"/>
+        <v>50</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="B3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="B4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="B5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="B6">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EFD4523-7F16-4EE5-BC77-7F896A2520B8}">
   <dimension ref="A1:X90"/>
   <sheetViews>
@@ -4024,7 +4354,7 @@
     </row>
     <row r="11" spans="1:24">
       <c r="A11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B11">
         <f ca="1">MOD(PRODUCT(E6:E10),G13)</f>
@@ -4087,7 +4417,7 @@
     </row>
     <row r="12" spans="1:24">
       <c r="A12" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B12">
         <f ca="1">MOD(B11*G11+G12,G13)</f>
@@ -4166,7 +4496,7 @@
     </row>
     <row r="13" spans="1:24">
       <c r="A13" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B13" s="41">
         <f t="shared" ref="B13:B33" ca="1" si="3">MOD(B12*G$11+G$12,G$13)</f>
@@ -4245,7 +4575,7 @@
     </row>
     <row r="14" spans="1:24">
       <c r="A14" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B14" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -4321,7 +4651,7 @@
     </row>
     <row r="15" spans="1:24">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B15" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -4397,7 +4727,7 @@
     </row>
     <row r="16" spans="1:24">
       <c r="A16" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B16" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -4473,7 +4803,7 @@
     </row>
     <row r="17" spans="1:24">
       <c r="A17" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B17" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -4549,7 +4879,7 @@
     </row>
     <row r="18" spans="1:24">
       <c r="A18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B18" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -4574,7 +4904,7 @@
     </row>
     <row r="19" spans="1:24">
       <c r="A19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B19" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -4599,7 +4929,7 @@
     </row>
     <row r="20" spans="1:24">
       <c r="A20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B20" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -4634,7 +4964,7 @@
     </row>
     <row r="21" spans="1:24">
       <c r="A21" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B21" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -4669,7 +4999,7 @@
     </row>
     <row r="22" spans="1:24">
       <c r="A22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B22" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -4705,7 +5035,7 @@
     </row>
     <row r="23" spans="1:24">
       <c r="A23" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B23" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -4741,7 +5071,7 @@
     </row>
     <row r="24" spans="1:24">
       <c r="A24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B24" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -4777,7 +5107,7 @@
     </row>
     <row r="25" spans="1:24">
       <c r="A25" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B25" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -4813,7 +5143,7 @@
     </row>
     <row r="26" spans="1:24">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B26" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -4849,7 +5179,7 @@
     </row>
     <row r="27" spans="1:24">
       <c r="A27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B27" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -4885,7 +5215,7 @@
     </row>
     <row r="28" spans="1:24">
       <c r="A28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B28" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -4921,7 +5251,7 @@
     </row>
     <row r="29" spans="1:24">
       <c r="A29" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B29" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -4957,7 +5287,7 @@
     </row>
     <row r="30" spans="1:24">
       <c r="A30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B30" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -4993,7 +5323,7 @@
     </row>
     <row r="31" spans="1:24">
       <c r="A31" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B31" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -5029,7 +5359,7 @@
     </row>
     <row r="32" spans="1:24">
       <c r="A32" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B32" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -5065,7 +5395,7 @@
     </row>
     <row r="33" spans="1:14">
       <c r="A33" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B33" s="41">
         <f t="shared" ca="1" si="3"/>
@@ -5101,7 +5431,7 @@
     </row>
     <row r="34" spans="1:14">
       <c r="A34" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B34" s="41">
         <f t="shared" ref="B34:B90" ca="1" si="9">MOD(B33*G$11+G$12,G$13)</f>
@@ -5136,7 +5466,7 @@
     </row>
     <row r="35" spans="1:14">
       <c r="A35" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B35" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5171,7 +5501,7 @@
     </row>
     <row r="36" spans="1:14">
       <c r="A36" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B36" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5206,7 +5536,7 @@
     </row>
     <row r="37" spans="1:14">
       <c r="A37" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B37" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5241,7 +5571,7 @@
     </row>
     <row r="38" spans="1:14">
       <c r="A38" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B38" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5276,7 +5606,7 @@
     </row>
     <row r="39" spans="1:14">
       <c r="A39" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B39" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5311,7 +5641,7 @@
     </row>
     <row r="40" spans="1:14">
       <c r="A40" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B40" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5346,7 +5676,7 @@
     </row>
     <row r="41" spans="1:14">
       <c r="A41" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B41" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5381,7 +5711,7 @@
     </row>
     <row r="42" spans="1:14">
       <c r="A42" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B42" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5416,7 +5746,7 @@
     </row>
     <row r="43" spans="1:14">
       <c r="A43" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B43" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5451,7 +5781,7 @@
     </row>
     <row r="44" spans="1:14">
       <c r="A44" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B44" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5486,7 +5816,7 @@
     </row>
     <row r="45" spans="1:14">
       <c r="A45" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B45" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5521,7 +5851,7 @@
     </row>
     <row r="46" spans="1:14">
       <c r="A46" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B46" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5556,7 +5886,7 @@
     </row>
     <row r="47" spans="1:14">
       <c r="A47" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B47" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5591,7 +5921,7 @@
     </row>
     <row r="48" spans="1:14">
       <c r="A48" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B48" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5626,7 +5956,7 @@
     </row>
     <row r="49" spans="1:11">
       <c r="A49" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B49" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5661,7 +5991,7 @@
     </row>
     <row r="50" spans="1:11">
       <c r="A50" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B50" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5696,7 +6026,7 @@
     </row>
     <row r="51" spans="1:11">
       <c r="A51" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B51" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5731,7 +6061,7 @@
     </row>
     <row r="52" spans="1:11">
       <c r="A52" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B52" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5766,7 +6096,7 @@
     </row>
     <row r="53" spans="1:11">
       <c r="A53" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B53" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5801,7 +6131,7 @@
     </row>
     <row r="54" spans="1:11">
       <c r="A54" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B54" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5836,7 +6166,7 @@
     </row>
     <row r="55" spans="1:11">
       <c r="A55" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B55" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5871,7 +6201,7 @@
     </row>
     <row r="56" spans="1:11">
       <c r="A56" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B56" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5906,7 +6236,7 @@
     </row>
     <row r="57" spans="1:11">
       <c r="A57" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B57" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5941,7 +6271,7 @@
     </row>
     <row r="58" spans="1:11">
       <c r="A58" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B58" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -5976,7 +6306,7 @@
     </row>
     <row r="59" spans="1:11">
       <c r="A59" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B59" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6011,7 +6341,7 @@
     </row>
     <row r="60" spans="1:11">
       <c r="A60" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B60" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6046,7 +6376,7 @@
     </row>
     <row r="61" spans="1:11">
       <c r="A61" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B61" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6081,7 +6411,7 @@
     </row>
     <row r="62" spans="1:11">
       <c r="A62" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B62" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6116,7 +6446,7 @@
     </row>
     <row r="63" spans="1:11">
       <c r="A63" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B63" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6151,7 +6481,7 @@
     </row>
     <row r="64" spans="1:11">
       <c r="A64" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B64" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6186,7 +6516,7 @@
     </row>
     <row r="65" spans="1:11">
       <c r="A65" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B65" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6221,7 +6551,7 @@
     </row>
     <row r="66" spans="1:11">
       <c r="A66" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B66" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6256,7 +6586,7 @@
     </row>
     <row r="67" spans="1:11">
       <c r="A67" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B67" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6291,7 +6621,7 @@
     </row>
     <row r="68" spans="1:11">
       <c r="A68" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B68" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6326,7 +6656,7 @@
     </row>
     <row r="69" spans="1:11">
       <c r="A69" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B69" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6361,7 +6691,7 @@
     </row>
     <row r="70" spans="1:11">
       <c r="A70" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B70" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6386,7 +6716,7 @@
     </row>
     <row r="71" spans="1:11">
       <c r="A71" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B71" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6411,7 +6741,7 @@
     </row>
     <row r="72" spans="1:11">
       <c r="A72" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B72" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6436,7 +6766,7 @@
     </row>
     <row r="73" spans="1:11">
       <c r="A73" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B73" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6461,7 +6791,7 @@
     </row>
     <row r="74" spans="1:11">
       <c r="A74" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B74" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6486,7 +6816,7 @@
     </row>
     <row r="75" spans="1:11">
       <c r="A75" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B75" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6511,7 +6841,7 @@
     </row>
     <row r="76" spans="1:11">
       <c r="A76" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B76" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6536,7 +6866,7 @@
     </row>
     <row r="77" spans="1:11">
       <c r="A77" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B77" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6561,7 +6891,7 @@
     </row>
     <row r="78" spans="1:11">
       <c r="A78" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B78" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6586,7 +6916,7 @@
     </row>
     <row r="79" spans="1:11">
       <c r="A79" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B79" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6611,7 +6941,7 @@
     </row>
     <row r="80" spans="1:11">
       <c r="A80" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B80" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6636,7 +6966,7 @@
     </row>
     <row r="81" spans="1:6">
       <c r="A81" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B81" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6661,7 +6991,7 @@
     </row>
     <row r="82" spans="1:6">
       <c r="A82" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B82" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6686,7 +7016,7 @@
     </row>
     <row r="83" spans="1:6">
       <c r="A83" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B83" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6711,7 +7041,7 @@
     </row>
     <row r="84" spans="1:6">
       <c r="A84" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B84" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6736,7 +7066,7 @@
     </row>
     <row r="85" spans="1:6">
       <c r="A85" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B85" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6761,7 +7091,7 @@
     </row>
     <row r="86" spans="1:6">
       <c r="A86" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B86" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6786,7 +7116,7 @@
     </row>
     <row r="87" spans="1:6">
       <c r="A87" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B87" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6811,7 +7141,7 @@
     </row>
     <row r="88" spans="1:6">
       <c r="A88" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B88" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6836,7 +7166,7 @@
     </row>
     <row r="89" spans="1:6">
       <c r="A89" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B89" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6861,7 +7191,7 @@
     </row>
     <row r="90" spans="1:6">
       <c r="A90" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B90" s="41">
         <f t="shared" ca="1" si="9"/>
@@ -6900,6 +7230,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002FC4D7A32A34E94B953742578E0D227D" ma:contentTypeVersion="15" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="6062e902822a1ea35e0b6c93f60576e5">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns3="d8c16f6f-632d-4fa9-9000-4a0cb55aa11b" xmlns:ns4="6588c10b-b5ed-4e95-9d69-08b9b2ce7055" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9a7d56c96ea3c0bda530556fd5715147" ns1:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -7139,15 +7478,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73BD24FA-A4D4-4F71-A18A-C8260E97BFC1}">
   <ds:schemaRefs>
@@ -7157,6 +7487,16 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23FC55F1-8C15-4A13-B875-E9240B3D0196}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7B51EC0E-1F4D-4A53-9313-26AAFAC23B23}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -7174,14 +7514,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23FC55F1-8C15-4A13-B875-E9240B3D0196}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Changed to decimal temps
</commit_message>
<xml_diff>
--- a/144F20/Topic 6/Topic 6 DQ 1 and 2.xlsx
+++ b/144F20/Topic 6/Topic 6 DQ 1 and 2.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gcumail-my.sharepoint.com/personal/richard_ketchersid_gcu_edu/Documents/Course Materials/git/Teaching/144F20/Topic 6/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="77" documentId="8_{A4867632-43AB-4763-8819-0561CF9679FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{79214B4B-1A7D-4A08-80A0-D6972B56B6C7}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="8_{A4867632-43AB-4763-8819-0561CF9679FB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{15AC572D-ED81-4219-9814-E3EDAF3B0D69}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="0" windowWidth="23010" windowHeight="12510" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12" yWindow="588" windowWidth="20112" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hand DQ1" sheetId="1" r:id="rId1"/>
@@ -1134,6 +1134,102 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
@@ -1169,15 +1265,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1186,93 +1273,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -1466,6 +1466,132 @@
             <a:rPr lang="en-US" sz="1100" b="1"/>
             <a:t>correctly.</a:t>
           </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="3957302" cy="781240"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="TextBox 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D716DF00-76B2-47D4-8EBD-1DADDE1B8CC0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7993380" y="2171700"/>
+          <a:ext cx="3957302" cy="781240"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent5">
+            <a:lumMod val="20000"/>
+            <a:lumOff val="80000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="none" rtlCol="0" anchor="t">
+          <a:spAutoFit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>There was confusion about bin</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>width and using decimals so after</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>the videos were made I changed this to use decimal temps. This is</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>important</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t> for understanding what is being done here. The videos</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+            </a:rPr>
+            <a:t>still apply.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100">
+            <a:solidFill>
+              <a:srgbClr val="FF0000"/>
+            </a:solidFill>
+          </a:endParaRPr>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -1877,84 +2003,84 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K56"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="1" max="1" width="17" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="13.6640625" customWidth="1"/>
     <col min="8" max="8" width="18" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
-    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
     <col min="11" max="11" width="21" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1">
-      <c r="D1" s="65" t="s">
+    <row r="1" spans="1:11" ht="15" thickBot="1">
+      <c r="D1" s="45" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="66"/>
-      <c r="F1" s="66"/>
-      <c r="G1" s="66"/>
-      <c r="H1" s="67"/>
+      <c r="E1" s="46"/>
+      <c r="F1" s="46"/>
+      <c r="G1" s="46"/>
+      <c r="H1" s="47"/>
     </row>
     <row r="2" spans="1:11" ht="18" thickBot="1">
       <c r="A2" s="42" t="s">
         <v>109</v>
       </c>
-      <c r="B2" s="63" t="s">
+      <c r="B2" s="43" t="s">
         <v>168</v>
       </c>
-      <c r="C2" s="64"/>
-      <c r="D2" s="68"/>
-      <c r="E2" s="69"/>
-      <c r="F2" s="69"/>
-      <c r="G2" s="69"/>
-      <c r="H2" s="70"/>
-    </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1">
-      <c r="D3" s="71"/>
-      <c r="E3" s="72"/>
-      <c r="F3" s="72"/>
-      <c r="G3" s="72"/>
-      <c r="H3" s="73"/>
-    </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1"/>
-    <row r="6" spans="1:11" ht="15.75">
+      <c r="C2" s="44"/>
+      <c r="D2" s="48"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="50"/>
+    </row>
+    <row r="3" spans="1:11" ht="15" thickBot="1">
+      <c r="D3" s="51"/>
+      <c r="E3" s="52"/>
+      <c r="F3" s="52"/>
+      <c r="G3" s="52"/>
+      <c r="H3" s="53"/>
+    </row>
+    <row r="5" spans="1:11" ht="15" thickBot="1"/>
+    <row r="6" spans="1:11" ht="15.6">
       <c r="A6" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D6" s="45" t="s">
+      <c r="D6" s="77" t="s">
         <v>63</v>
       </c>
-      <c r="E6" s="46"/>
-      <c r="F6" s="46"/>
-      <c r="G6" s="46"/>
-      <c r="H6" s="47"/>
-      <c r="J6" s="43" t="s">
+      <c r="E6" s="78"/>
+      <c r="F6" s="78"/>
+      <c r="G6" s="78"/>
+      <c r="H6" s="79"/>
+      <c r="J6" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="K6" s="44"/>
-    </row>
-    <row r="7" spans="1:11" ht="14.45" customHeight="1" thickBot="1">
+      <c r="K6" s="76"/>
+    </row>
+    <row r="7" spans="1:11" ht="14.4" customHeight="1" thickBot="1">
       <c r="A7" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B7" s="6">
         <f ca="1">Sheet1!K20</f>
-        <v>112</v>
-      </c>
-      <c r="D7" s="48"/>
-      <c r="E7" s="49"/>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="50"/>
+        <v>112.52</v>
+      </c>
+      <c r="D7" s="80"/>
+      <c r="E7" s="81"/>
+      <c r="F7" s="81"/>
+      <c r="G7" s="81"/>
+      <c r="H7" s="82"/>
       <c r="J7" s="7" t="s">
         <v>53</v>
       </c>
@@ -1962,13 +2088,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="14.45" customHeight="1" thickBot="1">
+    <row r="8" spans="1:11" ht="14.4" customHeight="1" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B8" s="6">
         <f ca="1">Sheet1!K21</f>
-        <v>100</v>
+        <v>100.13</v>
       </c>
       <c r="D8" s="15"/>
       <c r="E8" s="15"/>
@@ -1982,22 +2108,22 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="14.45" customHeight="1" thickBot="1">
+    <row r="9" spans="1:11" ht="14.4" customHeight="1" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B9" s="6">
         <f ca="1">Sheet1!K22</f>
-        <v>128</v>
+        <v>128.49</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="51" t="s">
+      <c r="D9" s="83" t="s">
         <v>65</v>
       </c>
-      <c r="E9" s="52"/>
-      <c r="F9" s="53"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="85"/>
       <c r="G9" s="39" t="s">
         <v>84</v>
       </c>
@@ -2009,22 +2135,22 @@
         <v>58</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1">
+    <row r="10" spans="1:11" ht="15" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>14</v>
       </c>
       <c r="B10" s="6">
         <f ca="1">Sheet1!K23</f>
-        <v>120</v>
+        <v>120.74</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="D10" s="51" t="s">
+      <c r="D10" s="83" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="52"/>
-      <c r="F10" s="53"/>
+      <c r="E10" s="84"/>
+      <c r="F10" s="85"/>
       <c r="G10" s="18"/>
       <c r="H10" s="40" t="s">
         <v>84</v>
@@ -2042,16 +2168,16 @@
       </c>
       <c r="B11" s="6">
         <f ca="1">Sheet1!K24</f>
-        <v>142</v>
+        <v>142.01</v>
       </c>
       <c r="C11" s="16"/>
-      <c r="D11" s="74" t="s">
+      <c r="D11" s="60" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="75"/>
-      <c r="F11" s="75"/>
-      <c r="G11" s="75"/>
-      <c r="H11" s="76"/>
+      <c r="E11" s="61"/>
+      <c r="F11" s="61"/>
+      <c r="G11" s="61"/>
+      <c r="H11" s="62"/>
       <c r="J11" s="13" t="s">
         <v>61</v>
       </c>
@@ -2065,13 +2191,13 @@
       </c>
       <c r="B12" s="6">
         <f ca="1">Sheet1!K25</f>
-        <v>118</v>
-      </c>
-      <c r="D12" s="77"/>
-      <c r="E12" s="78"/>
-      <c r="F12" s="78"/>
-      <c r="G12" s="78"/>
-      <c r="H12" s="79"/>
+        <v>118.38</v>
+      </c>
+      <c r="D12" s="63"/>
+      <c r="E12" s="64"/>
+      <c r="F12" s="64"/>
+      <c r="G12" s="64"/>
+      <c r="H12" s="65"/>
     </row>
     <row r="13" spans="1:11">
       <c r="A13" s="5" t="s">
@@ -2079,65 +2205,65 @@
       </c>
       <c r="B13" s="6">
         <f ca="1">Sheet1!K26</f>
-        <v>106</v>
-      </c>
-      <c r="D13" s="77"/>
-      <c r="E13" s="78"/>
-      <c r="F13" s="78"/>
-      <c r="G13" s="78"/>
-      <c r="H13" s="79"/>
-    </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1">
+        <v>106.86</v>
+      </c>
+      <c r="D13" s="63"/>
+      <c r="E13" s="64"/>
+      <c r="F13" s="64"/>
+      <c r="G13" s="64"/>
+      <c r="H13" s="65"/>
+    </row>
+    <row r="14" spans="1:11" ht="15" thickBot="1">
       <c r="A14" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B14" s="6">
         <f ca="1">Sheet1!K27</f>
-        <v>110</v>
-      </c>
-      <c r="D14" s="80"/>
-      <c r="E14" s="81"/>
-      <c r="F14" s="81"/>
-      <c r="G14" s="81"/>
-      <c r="H14" s="82"/>
-    </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1">
+        <v>110.76</v>
+      </c>
+      <c r="D14" s="66"/>
+      <c r="E14" s="67"/>
+      <c r="F14" s="67"/>
+      <c r="G14" s="67"/>
+      <c r="H14" s="68"/>
+    </row>
+    <row r="15" spans="1:11" ht="15" thickBot="1">
       <c r="A15" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B15" s="6">
         <f ca="1">Sheet1!K28</f>
-        <v>114</v>
+        <v>114.66</v>
       </c>
       <c r="C15" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D15" s="83" t="s">
+      <c r="D15" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="84"/>
-      <c r="F15" s="85"/>
+      <c r="E15" s="70"/>
+      <c r="F15" s="71"/>
       <c r="G15" s="18"/>
       <c r="H15" s="40" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1">
+    <row r="16" spans="1:11" ht="15" thickBot="1">
       <c r="A16" s="5" t="s">
         <v>45</v>
       </c>
       <c r="B16" s="6">
         <f ca="1">Sheet1!K29</f>
-        <v>112</v>
+        <v>112.59</v>
       </c>
       <c r="C16" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="D16" s="86" t="s">
+      <c r="D16" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="E16" s="87"/>
-      <c r="F16" s="88"/>
+      <c r="E16" s="73"/>
+      <c r="F16" s="74"/>
       <c r="G16" s="40" t="s">
         <v>84</v>
       </c>
@@ -2149,7 +2275,7 @@
       </c>
       <c r="B17" s="6">
         <f ca="1">Sheet1!K30</f>
-        <v>95</v>
+        <v>95.62</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>73</v>
@@ -2173,7 +2299,7 @@
       </c>
       <c r="B18" s="6">
         <f ca="1">Sheet1!K31</f>
-        <v>125</v>
+        <v>125.29</v>
       </c>
       <c r="D18" s="1">
         <v>1</v>
@@ -2189,7 +2315,7 @@
       </c>
       <c r="B19" s="6">
         <f ca="1">Sheet1!K32</f>
-        <v>117</v>
+        <v>117.3</v>
       </c>
       <c r="D19" s="1">
         <v>2</v>
@@ -2206,7 +2332,7 @@
       </c>
       <c r="B20" s="6">
         <f ca="1">Sheet1!K33</f>
-        <v>112</v>
+        <v>112.74</v>
       </c>
       <c r="D20" s="1">
         <v>3</v>
@@ -2222,7 +2348,7 @@
       </c>
       <c r="B21" s="6">
         <f ca="1">Sheet1!K34</f>
-        <v>118</v>
+        <v>118.35</v>
       </c>
       <c r="D21" s="1">
         <v>4</v>
@@ -2238,7 +2364,7 @@
       </c>
       <c r="B22" s="6">
         <f ca="1">Sheet1!K35</f>
-        <v>121</v>
+        <v>121.05</v>
       </c>
       <c r="D22" s="1">
         <v>5</v>
@@ -2248,13 +2374,13 @@
       <c r="G22" s="23"/>
       <c r="H22" s="23"/>
     </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1">
+    <row r="23" spans="1:11" ht="15" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>11</v>
       </c>
       <c r="B23" s="6">
         <f ca="1">Sheet1!K36</f>
-        <v>114</v>
+        <v>114.27</v>
       </c>
       <c r="D23" s="1">
         <v>6</v>
@@ -2264,13 +2390,13 @@
       <c r="G23" s="24"/>
       <c r="H23" s="24"/>
     </row>
-    <row r="24" spans="1:11" ht="14.45" customHeight="1">
+    <row r="24" spans="1:11" ht="14.4" customHeight="1">
       <c r="A24" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B24" s="6">
         <f ca="1">Sheet1!K37</f>
-        <v>114</v>
+        <v>114.29</v>
       </c>
       <c r="C24" s="16"/>
       <c r="D24" s="54" t="s">
@@ -2287,13 +2413,13 @@
       </c>
       <c r="B25" s="6">
         <f ca="1">Sheet1!K38</f>
-        <v>111</v>
-      </c>
-      <c r="D25" s="57"/>
-      <c r="E25" s="58"/>
-      <c r="F25" s="58"/>
-      <c r="G25" s="58"/>
-      <c r="H25" s="59"/>
+        <v>111.14</v>
+      </c>
+      <c r="D25" s="86"/>
+      <c r="E25" s="87"/>
+      <c r="F25" s="87"/>
+      <c r="G25" s="87"/>
+      <c r="H25" s="88"/>
     </row>
     <row r="26" spans="1:11">
       <c r="A26" s="5" t="s">
@@ -2301,27 +2427,27 @@
       </c>
       <c r="B26" s="6">
         <f ca="1">Sheet1!K39</f>
-        <v>109</v>
-      </c>
-      <c r="D26" s="57"/>
-      <c r="E26" s="58"/>
-      <c r="F26" s="58"/>
-      <c r="G26" s="58"/>
-      <c r="H26" s="59"/>
-    </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1">
+        <v>109.26</v>
+      </c>
+      <c r="D26" s="86"/>
+      <c r="E26" s="87"/>
+      <c r="F26" s="87"/>
+      <c r="G26" s="87"/>
+      <c r="H26" s="88"/>
+    </row>
+    <row r="27" spans="1:11" ht="15" thickBot="1">
       <c r="A27" s="5" t="s">
         <v>17</v>
       </c>
       <c r="B27" s="6">
         <f ca="1">Sheet1!K40</f>
-        <v>104</v>
-      </c>
-      <c r="D27" s="60"/>
-      <c r="E27" s="61"/>
-      <c r="F27" s="61"/>
-      <c r="G27" s="61"/>
-      <c r="H27" s="62"/>
+        <v>104.41</v>
+      </c>
+      <c r="D27" s="57"/>
+      <c r="E27" s="58"/>
+      <c r="F27" s="58"/>
+      <c r="G27" s="58"/>
+      <c r="H27" s="59"/>
     </row>
     <row r="28" spans="1:11">
       <c r="A28" s="5" t="s">
@@ -2329,7 +2455,7 @@
       </c>
       <c r="B28" s="6">
         <f ca="1">Sheet1!K41</f>
-        <v>119</v>
+        <v>119.21</v>
       </c>
       <c r="C28" s="16" t="s">
         <v>78</v>
@@ -2345,19 +2471,19 @@
         <v>84</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.75" thickBot="1">
+    <row r="29" spans="1:11" ht="15" thickBot="1">
       <c r="A29" s="5" t="s">
         <v>48</v>
       </c>
       <c r="B29" s="6">
         <f ca="1">Sheet1!K42</f>
-        <v>114</v>
-      </c>
-      <c r="D29" s="60"/>
-      <c r="E29" s="61"/>
-      <c r="F29" s="61"/>
-      <c r="G29" s="61"/>
-      <c r="H29" s="62"/>
+        <v>114.6</v>
+      </c>
+      <c r="D29" s="57"/>
+      <c r="E29" s="58"/>
+      <c r="F29" s="58"/>
+      <c r="G29" s="58"/>
+      <c r="H29" s="59"/>
     </row>
     <row r="30" spans="1:11">
       <c r="A30" s="5" t="s">
@@ -2365,7 +2491,7 @@
       </c>
       <c r="B30" s="6">
         <f ca="1">Sheet1!K43</f>
-        <v>115</v>
+        <v>115.64</v>
       </c>
       <c r="E30" s="2"/>
       <c r="H30" s="2"/>
@@ -2376,7 +2502,7 @@
       </c>
       <c r="B31" s="6">
         <f ca="1">Sheet1!K44</f>
-        <v>118</v>
+        <v>118.08</v>
       </c>
       <c r="C31">
         <v>20</v>
@@ -2394,7 +2520,7 @@
       </c>
       <c r="B32" s="6">
         <f ca="1">Sheet1!K45</f>
-        <v>117</v>
+        <v>117.98</v>
       </c>
       <c r="C32">
         <v>19</v>
@@ -2412,7 +2538,7 @@
       </c>
       <c r="B33" s="6">
         <f ca="1">Sheet1!K46</f>
-        <v>118</v>
+        <v>118.82</v>
       </c>
       <c r="C33">
         <v>18</v>
@@ -2430,7 +2556,7 @@
       </c>
       <c r="B34" s="6">
         <f ca="1">Sheet1!K47</f>
-        <v>125</v>
+        <v>125.41</v>
       </c>
       <c r="C34">
         <v>17</v>
@@ -2448,7 +2574,7 @@
       </c>
       <c r="B35" s="6">
         <f ca="1">Sheet1!K48</f>
-        <v>106</v>
+        <v>106.12</v>
       </c>
       <c r="C35">
         <v>16</v>
@@ -2466,7 +2592,7 @@
       </c>
       <c r="B36" s="6">
         <f ca="1">Sheet1!K49</f>
-        <v>108</v>
+        <v>108.56</v>
       </c>
       <c r="C36">
         <v>15</v>
@@ -2484,7 +2610,7 @@
       </c>
       <c r="B37" s="6">
         <f ca="1">Sheet1!K50</f>
-        <v>122</v>
+        <v>122.38</v>
       </c>
       <c r="C37">
         <v>14</v>
@@ -2502,7 +2628,7 @@
       </c>
       <c r="B38" s="6">
         <f ca="1">Sheet1!K51</f>
-        <v>114</v>
+        <v>114.29</v>
       </c>
       <c r="C38">
         <v>13</v>
@@ -2520,7 +2646,7 @@
       </c>
       <c r="B39" s="6">
         <f ca="1">Sheet1!K52</f>
-        <v>109</v>
+        <v>109.86</v>
       </c>
       <c r="C39" s="32">
         <v>12</v>
@@ -2538,7 +2664,7 @@
       </c>
       <c r="B40" s="6">
         <f ca="1">Sheet1!K53</f>
-        <v>121</v>
+        <v>121.42</v>
       </c>
       <c r="C40">
         <v>11</v>
@@ -2556,7 +2682,7 @@
       </c>
       <c r="B41" s="6">
         <f ca="1">Sheet1!K54</f>
-        <v>121</v>
+        <v>121.39</v>
       </c>
       <c r="C41">
         <v>10</v>
@@ -2574,7 +2700,7 @@
       </c>
       <c r="B42" s="6">
         <f ca="1">Sheet1!K55</f>
-        <v>120</v>
+        <v>120.49</v>
       </c>
       <c r="C42">
         <v>9</v>
@@ -2592,7 +2718,7 @@
       </c>
       <c r="B43" s="6">
         <f ca="1">Sheet1!K56</f>
-        <v>118</v>
+        <v>118.16</v>
       </c>
       <c r="C43">
         <v>8</v>
@@ -2610,7 +2736,7 @@
       </c>
       <c r="B44" s="6">
         <f ca="1">Sheet1!K57</f>
-        <v>117</v>
+        <v>117.52</v>
       </c>
       <c r="C44">
         <v>7</v>
@@ -2628,7 +2754,7 @@
       </c>
       <c r="B45" s="6">
         <f ca="1">Sheet1!K58</f>
-        <v>104</v>
+        <v>104.44</v>
       </c>
       <c r="C45">
         <v>6</v>
@@ -2646,7 +2772,7 @@
       </c>
       <c r="B46" s="6">
         <f ca="1">Sheet1!K59</f>
-        <v>110</v>
+        <v>110.74</v>
       </c>
       <c r="C46">
         <v>5</v>
@@ -2664,7 +2790,7 @@
       </c>
       <c r="B47" s="6">
         <f ca="1">Sheet1!K60</f>
-        <v>129</v>
+        <v>129.35</v>
       </c>
       <c r="C47">
         <v>4</v>
@@ -2682,7 +2808,7 @@
       </c>
       <c r="B48" s="6">
         <f ca="1">Sheet1!K61</f>
-        <v>113</v>
+        <v>113.34</v>
       </c>
       <c r="C48">
         <v>3</v>
@@ -2700,7 +2826,7 @@
       </c>
       <c r="B49" s="6">
         <f ca="1">Sheet1!K62</f>
-        <v>120</v>
+        <v>120.61</v>
       </c>
       <c r="C49">
         <v>2</v>
@@ -2712,13 +2838,13 @@
       <c r="H49" s="2"/>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" ht="15.75" thickBot="1">
+    <row r="50" spans="1:9" ht="15" thickBot="1">
       <c r="A50" s="5" t="s">
         <v>16</v>
       </c>
       <c r="B50" s="6">
         <f ca="1">Sheet1!K63</f>
-        <v>117</v>
+        <v>117.25</v>
       </c>
       <c r="C50">
         <v>1</v>
@@ -2730,13 +2856,13 @@
       <c r="H50" s="25"/>
       <c r="I50" s="25"/>
     </row>
-    <row r="51" spans="1:9" ht="15.75" thickTop="1">
+    <row r="51" spans="1:9" ht="15" thickTop="1">
       <c r="A51" s="5" t="s">
         <v>28</v>
       </c>
       <c r="B51" s="6">
         <f ca="1">Sheet1!K64</f>
-        <v>103</v>
+        <v>103.28</v>
       </c>
       <c r="E51" s="2"/>
       <c r="H51" s="2"/>
@@ -2747,7 +2873,7 @@
       </c>
       <c r="B52" s="6">
         <f ca="1">Sheet1!K65</f>
-        <v>115</v>
+        <v>115.85</v>
       </c>
       <c r="E52" s="2"/>
       <c r="H52" s="2"/>
@@ -2758,7 +2884,7 @@
       </c>
       <c r="B53" s="6">
         <f ca="1">Sheet1!K66</f>
-        <v>114</v>
+        <v>114.51</v>
       </c>
       <c r="E53" s="2"/>
       <c r="H53" s="2"/>
@@ -2769,7 +2895,7 @@
       </c>
       <c r="B54" s="6">
         <f ca="1">Sheet1!K67</f>
-        <v>119</v>
+        <v>119.75</v>
       </c>
       <c r="E54" s="2"/>
       <c r="H54" s="2"/>
@@ -2780,7 +2906,7 @@
       </c>
       <c r="B55" s="6">
         <f ca="1">Sheet1!K68</f>
-        <v>114</v>
+        <v>114.3</v>
       </c>
       <c r="E55" s="2"/>
       <c r="H55" s="2"/>
@@ -2791,7 +2917,7 @@
       </c>
       <c r="B56" s="6">
         <f ca="1">Sheet1!K69</f>
-        <v>112</v>
+        <v>112.51</v>
       </c>
       <c r="E56" s="2"/>
       <c r="H56" s="2"/>
@@ -2801,17 +2927,17 @@
     <sortCondition ref="A7:A57"/>
   </sortState>
   <mergeCells count="11">
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="D6:H7"/>
+    <mergeCell ref="D9:F9"/>
+    <mergeCell ref="D10:F10"/>
+    <mergeCell ref="D24:H27"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="D1:H3"/>
     <mergeCell ref="D28:H29"/>
     <mergeCell ref="D11:H14"/>
     <mergeCell ref="D15:F15"/>
     <mergeCell ref="D16:F16"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="D6:H7"/>
-    <mergeCell ref="D9:F9"/>
-    <mergeCell ref="D10:F10"/>
-    <mergeCell ref="D24:H27"/>
   </mergeCells>
   <conditionalFormatting sqref="A5:K56">
     <cfRule type="expression" dxfId="3" priority="2">
@@ -2854,22 +2980,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A1137E8F-1C1D-4812-96CD-8ACE7317344E}">
   <dimension ref="A1:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J21" sqref="J21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16.42578125" customWidth="1"/>
-    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="7" width="13.6640625" customWidth="1"/>
+    <col min="8" max="8" width="16.44140625" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" customWidth="1"/>
     <col min="10" max="10" width="16" customWidth="1"/>
-    <col min="11" max="11" width="21.140625" customWidth="1"/>
+    <col min="11" max="11" width="21.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75">
+    <row r="1" spans="1:11" ht="15.6">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -2883,18 +3009,18 @@
       <c r="F1" s="97"/>
       <c r="G1" s="97"/>
       <c r="H1" s="98"/>
-      <c r="J1" s="43" t="s">
+      <c r="J1" s="75" t="s">
         <v>52</v>
       </c>
-      <c r="K1" s="44"/>
-    </row>
-    <row r="2" spans="1:11" ht="14.45" customHeight="1" thickBot="1">
+      <c r="K1" s="76"/>
+    </row>
+    <row r="2" spans="1:11" ht="14.4" customHeight="1" thickBot="1">
       <c r="A2" s="5" t="s">
         <v>29</v>
       </c>
       <c r="B2" s="6">
         <f ca="1">Sheet1!K20</f>
-        <v>112</v>
+        <v>112.52</v>
       </c>
       <c r="D2" s="99"/>
       <c r="E2" s="100"/>
@@ -2908,13 +3034,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="14.45" customHeight="1" thickBot="1">
+    <row r="3" spans="1:11" ht="14.4" customHeight="1" thickBot="1">
       <c r="A3" s="5" t="s">
         <v>27</v>
       </c>
       <c r="B3" s="6">
         <f ca="1">Sheet1!K21</f>
-        <v>100</v>
+        <v>100.13</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15"/>
@@ -2928,13 +3054,13 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="14.45" customHeight="1" thickBot="1">
+    <row r="4" spans="1:11" ht="14.4" customHeight="1" thickBot="1">
       <c r="A4" s="5" t="s">
         <v>44</v>
       </c>
       <c r="B4" s="6">
         <f ca="1">Sheet1!K22</f>
-        <v>128</v>
+        <v>128.49</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>64</v>
@@ -2961,7 +3087,7 @@
       </c>
       <c r="B5" s="6">
         <f ca="1">Sheet1!K23</f>
-        <v>120</v>
+        <v>120.74</v>
       </c>
       <c r="C5" s="16"/>
       <c r="D5" s="54" t="s">
@@ -2984,13 +3110,13 @@
       </c>
       <c r="B6" s="6">
         <f ca="1">Sheet1!K24</f>
-        <v>142</v>
-      </c>
-      <c r="D6" s="57"/>
-      <c r="E6" s="58"/>
-      <c r="F6" s="58"/>
-      <c r="G6" s="58"/>
-      <c r="H6" s="59"/>
+        <v>142.01</v>
+      </c>
+      <c r="D6" s="86"/>
+      <c r="E6" s="87"/>
+      <c r="F6" s="87"/>
+      <c r="G6" s="87"/>
+      <c r="H6" s="88"/>
       <c r="J6" s="13" t="s">
         <v>61</v>
       </c>
@@ -3004,65 +3130,65 @@
       </c>
       <c r="B7" s="6">
         <f ca="1">Sheet1!K25</f>
-        <v>118</v>
-      </c>
-      <c r="D7" s="57"/>
-      <c r="E7" s="58"/>
-      <c r="F7" s="58"/>
-      <c r="G7" s="58"/>
-      <c r="H7" s="59"/>
-    </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1">
+        <v>118.38</v>
+      </c>
+      <c r="D7" s="86"/>
+      <c r="E7" s="87"/>
+      <c r="F7" s="87"/>
+      <c r="G7" s="87"/>
+      <c r="H7" s="88"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" thickBot="1">
       <c r="A8" s="5" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="6">
         <f ca="1">Sheet1!K26</f>
-        <v>106</v>
-      </c>
-      <c r="D8" s="60"/>
-      <c r="E8" s="61"/>
-      <c r="F8" s="61"/>
-      <c r="G8" s="61"/>
-      <c r="H8" s="62"/>
-    </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1">
+        <v>106.86</v>
+      </c>
+      <c r="D8" s="57"/>
+      <c r="E8" s="58"/>
+      <c r="F8" s="58"/>
+      <c r="G8" s="58"/>
+      <c r="H8" s="59"/>
+    </row>
+    <row r="9" spans="1:11" ht="15" thickBot="1">
       <c r="A9" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B9" s="6">
         <f ca="1">Sheet1!K27</f>
-        <v>110</v>
+        <v>110.76</v>
       </c>
       <c r="C9" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="83" t="s">
+      <c r="D9" s="69" t="s">
         <v>70</v>
       </c>
-      <c r="E9" s="84"/>
-      <c r="F9" s="85"/>
+      <c r="E9" s="70"/>
+      <c r="F9" s="71"/>
       <c r="G9" s="35"/>
       <c r="H9" s="40" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1">
+    <row r="10" spans="1:11" ht="15" thickBot="1">
       <c r="A10" s="5" t="s">
         <v>30</v>
       </c>
       <c r="B10" s="6">
         <f ca="1">Sheet1!K28</f>
-        <v>114</v>
+        <v>114.66</v>
       </c>
       <c r="C10" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="86" t="s">
+      <c r="D10" s="72" t="s">
         <v>72</v>
       </c>
-      <c r="E10" s="87"/>
-      <c r="F10" s="88"/>
+      <c r="E10" s="73"/>
+      <c r="F10" s="74"/>
       <c r="G10" s="40" t="s">
         <v>84</v>
       </c>
@@ -3078,7 +3204,7 @@
       </c>
       <c r="B11" s="6">
         <f ca="1">Sheet1!K29</f>
-        <v>112</v>
+        <v>112.59</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>73</v>
@@ -3107,7 +3233,7 @@
       </c>
       <c r="B12" s="6">
         <f ca="1">Sheet1!K30</f>
-        <v>95</v>
+        <v>95.62</v>
       </c>
       <c r="D12" s="1">
         <v>1</v>
@@ -3123,7 +3249,7 @@
       </c>
       <c r="B13" s="6">
         <f ca="1">Sheet1!K31</f>
-        <v>125</v>
+        <v>125.29</v>
       </c>
       <c r="D13" s="1">
         <v>2</v>
@@ -3139,7 +3265,7 @@
       </c>
       <c r="B14" s="6">
         <f ca="1">Sheet1!K32</f>
-        <v>117</v>
+        <v>117.3</v>
       </c>
       <c r="D14" s="1">
         <v>3</v>
@@ -3155,7 +3281,7 @@
       </c>
       <c r="B15" s="6">
         <f ca="1">Sheet1!K33</f>
-        <v>112</v>
+        <v>112.74</v>
       </c>
       <c r="D15" s="1">
         <v>4</v>
@@ -3171,7 +3297,7 @@
       </c>
       <c r="B16" s="6">
         <f ca="1">Sheet1!K34</f>
-        <v>118</v>
+        <v>118.35</v>
       </c>
       <c r="D16" s="1">
         <v>5</v>
@@ -3181,13 +3307,13 @@
       <c r="G16" s="36"/>
       <c r="H16" s="36"/>
     </row>
-    <row r="17" spans="1:9" ht="15.75" thickBot="1">
+    <row r="17" spans="1:9" ht="15" thickBot="1">
       <c r="A17" s="5" t="s">
         <v>40</v>
       </c>
       <c r="B17" s="6">
         <f ca="1">Sheet1!K35</f>
-        <v>121</v>
+        <v>121.05</v>
       </c>
       <c r="D17" s="1">
         <v>6</v>
@@ -3203,7 +3329,7 @@
       </c>
       <c r="B18" s="6">
         <f ca="1">Sheet1!K36</f>
-        <v>114</v>
+        <v>114.27</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="54" t="s">
@@ -3214,19 +3340,19 @@
       <c r="G18" s="55"/>
       <c r="H18" s="56"/>
     </row>
-    <row r="19" spans="1:9" ht="14.45" customHeight="1">
+    <row r="19" spans="1:9" ht="14.4" customHeight="1">
       <c r="A19" s="5" t="s">
         <v>5</v>
       </c>
       <c r="B19" s="6">
         <f ca="1">Sheet1!K37</f>
-        <v>114</v>
-      </c>
-      <c r="D19" s="57"/>
-      <c r="E19" s="58"/>
-      <c r="F19" s="58"/>
-      <c r="G19" s="58"/>
-      <c r="H19" s="59"/>
+        <v>114.29</v>
+      </c>
+      <c r="D19" s="86"/>
+      <c r="E19" s="87"/>
+      <c r="F19" s="87"/>
+      <c r="G19" s="87"/>
+      <c r="H19" s="88"/>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" s="5" t="s">
@@ -3234,27 +3360,27 @@
       </c>
       <c r="B20" s="6">
         <f ca="1">Sheet1!K38</f>
-        <v>111</v>
-      </c>
-      <c r="D20" s="57"/>
-      <c r="E20" s="58"/>
-      <c r="F20" s="58"/>
-      <c r="G20" s="58"/>
-      <c r="H20" s="59"/>
-    </row>
-    <row r="21" spans="1:9" ht="15.75" thickBot="1">
+        <v>111.14</v>
+      </c>
+      <c r="D20" s="86"/>
+      <c r="E20" s="87"/>
+      <c r="F20" s="87"/>
+      <c r="G20" s="87"/>
+      <c r="H20" s="88"/>
+    </row>
+    <row r="21" spans="1:9" ht="15" thickBot="1">
       <c r="A21" s="5" t="s">
         <v>50</v>
       </c>
       <c r="B21" s="6">
         <f ca="1">Sheet1!K39</f>
-        <v>109</v>
-      </c>
-      <c r="D21" s="60"/>
-      <c r="E21" s="61"/>
-      <c r="F21" s="61"/>
-      <c r="G21" s="61"/>
-      <c r="H21" s="62"/>
+        <v>109.26</v>
+      </c>
+      <c r="D21" s="57"/>
+      <c r="E21" s="58"/>
+      <c r="F21" s="58"/>
+      <c r="G21" s="58"/>
+      <c r="H21" s="59"/>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" s="5" t="s">
@@ -3262,7 +3388,7 @@
       </c>
       <c r="B22" s="6">
         <f ca="1">Sheet1!K40</f>
-        <v>104</v>
+        <v>104.41</v>
       </c>
       <c r="C22" s="16" t="s">
         <v>71</v>
@@ -3278,13 +3404,13 @@
         <v>84</v>
       </c>
     </row>
-    <row r="23" spans="1:9" ht="15.75" thickBot="1">
+    <row r="23" spans="1:9" ht="15" thickBot="1">
       <c r="A23" s="5" t="s">
         <v>10</v>
       </c>
       <c r="B23" s="6">
         <f ca="1">Sheet1!K41</f>
-        <v>119</v>
+        <v>119.21</v>
       </c>
       <c r="D23" s="92"/>
       <c r="E23" s="93"/>
@@ -3298,7 +3424,7 @@
       </c>
       <c r="B24" s="6">
         <f ca="1">Sheet1!K42</f>
-        <v>114</v>
+        <v>114.6</v>
       </c>
       <c r="E24" s="2"/>
       <c r="H24" s="2"/>
@@ -3309,7 +3435,7 @@
       </c>
       <c r="B25" s="6">
         <f ca="1">Sheet1!K43</f>
-        <v>115</v>
+        <v>115.64</v>
       </c>
       <c r="E25" s="2"/>
       <c r="H25" s="2"/>
@@ -3320,7 +3446,7 @@
       </c>
       <c r="B26" s="6">
         <f ca="1">Sheet1!K44</f>
-        <v>118</v>
+        <v>118.08</v>
       </c>
       <c r="E26" s="2"/>
       <c r="H26" s="2"/>
@@ -3332,7 +3458,7 @@
       </c>
       <c r="B27" s="6">
         <f ca="1">Sheet1!K45</f>
-        <v>117</v>
+        <v>117.98</v>
       </c>
       <c r="E27" s="2"/>
       <c r="H27" s="2"/>
@@ -3343,7 +3469,7 @@
       </c>
       <c r="B28" s="6">
         <f ca="1">Sheet1!K46</f>
-        <v>118</v>
+        <v>118.82</v>
       </c>
       <c r="E28" s="2"/>
       <c r="H28" s="2"/>
@@ -3354,7 +3480,7 @@
       </c>
       <c r="B29" s="6">
         <f ca="1">Sheet1!K47</f>
-        <v>125</v>
+        <v>125.41</v>
       </c>
     </row>
     <row r="30" spans="1:9">
@@ -3363,7 +3489,7 @@
       </c>
       <c r="B30" s="6">
         <f ca="1">Sheet1!K48</f>
-        <v>106</v>
+        <v>106.12</v>
       </c>
     </row>
     <row r="31" spans="1:9">
@@ -3372,7 +3498,7 @@
       </c>
       <c r="B31" s="6">
         <f ca="1">Sheet1!K49</f>
-        <v>108</v>
+        <v>108.56</v>
       </c>
     </row>
     <row r="32" spans="1:9">
@@ -3381,7 +3507,7 @@
       </c>
       <c r="B32" s="6">
         <f ca="1">Sheet1!K50</f>
-        <v>122</v>
+        <v>122.38</v>
       </c>
     </row>
     <row r="33" spans="1:3">
@@ -3390,7 +3516,7 @@
       </c>
       <c r="B33" s="6">
         <f ca="1">Sheet1!K51</f>
-        <v>114</v>
+        <v>114.29</v>
       </c>
       <c r="C33" s="32"/>
     </row>
@@ -3400,7 +3526,7 @@
       </c>
       <c r="B34" s="6">
         <f ca="1">Sheet1!K52</f>
-        <v>109</v>
+        <v>109.86</v>
       </c>
     </row>
     <row r="35" spans="1:3">
@@ -3409,7 +3535,7 @@
       </c>
       <c r="B35" s="6">
         <f ca="1">Sheet1!K53</f>
-        <v>121</v>
+        <v>121.42</v>
       </c>
     </row>
     <row r="36" spans="1:3">
@@ -3418,7 +3544,7 @@
       </c>
       <c r="B36" s="6">
         <f ca="1">Sheet1!K54</f>
-        <v>121</v>
+        <v>121.39</v>
       </c>
     </row>
     <row r="37" spans="1:3">
@@ -3427,7 +3553,7 @@
       </c>
       <c r="B37" s="6">
         <f ca="1">Sheet1!K55</f>
-        <v>120</v>
+        <v>120.49</v>
       </c>
     </row>
     <row r="38" spans="1:3">
@@ -3436,7 +3562,7 @@
       </c>
       <c r="B38" s="6">
         <f ca="1">Sheet1!K56</f>
-        <v>118</v>
+        <v>118.16</v>
       </c>
     </row>
     <row r="39" spans="1:3">
@@ -3445,7 +3571,7 @@
       </c>
       <c r="B39" s="6">
         <f ca="1">Sheet1!K57</f>
-        <v>117</v>
+        <v>117.52</v>
       </c>
     </row>
     <row r="40" spans="1:3">
@@ -3454,7 +3580,7 @@
       </c>
       <c r="B40" s="6">
         <f ca="1">Sheet1!K58</f>
-        <v>104</v>
+        <v>104.44</v>
       </c>
     </row>
     <row r="41" spans="1:3">
@@ -3463,7 +3589,7 @@
       </c>
       <c r="B41" s="6">
         <f ca="1">Sheet1!K59</f>
-        <v>110</v>
+        <v>110.74</v>
       </c>
     </row>
     <row r="42" spans="1:3">
@@ -3472,7 +3598,7 @@
       </c>
       <c r="B42" s="6">
         <f ca="1">Sheet1!K60</f>
-        <v>129</v>
+        <v>129.35</v>
       </c>
     </row>
     <row r="43" spans="1:3">
@@ -3481,7 +3607,7 @@
       </c>
       <c r="B43" s="6">
         <f ca="1">Sheet1!K61</f>
-        <v>113</v>
+        <v>113.34</v>
       </c>
     </row>
     <row r="44" spans="1:3">
@@ -3490,7 +3616,7 @@
       </c>
       <c r="B44" s="6">
         <f ca="1">Sheet1!K62</f>
-        <v>120</v>
+        <v>120.61</v>
       </c>
     </row>
     <row r="45" spans="1:3">
@@ -3499,7 +3625,7 @@
       </c>
       <c r="B45" s="6">
         <f ca="1">Sheet1!K63</f>
-        <v>117</v>
+        <v>117.25</v>
       </c>
     </row>
     <row r="46" spans="1:3">
@@ -3508,7 +3634,7 @@
       </c>
       <c r="B46" s="6">
         <f ca="1">Sheet1!K64</f>
-        <v>103</v>
+        <v>103.28</v>
       </c>
     </row>
     <row r="47" spans="1:3">
@@ -3517,7 +3643,7 @@
       </c>
       <c r="B47" s="6">
         <f ca="1">Sheet1!K65</f>
-        <v>115</v>
+        <v>115.85</v>
       </c>
     </row>
     <row r="48" spans="1:3">
@@ -3526,7 +3652,7 @@
       </c>
       <c r="B48" s="6">
         <f ca="1">Sheet1!K66</f>
-        <v>114</v>
+        <v>114.51</v>
       </c>
     </row>
     <row r="49" spans="1:2">
@@ -3535,7 +3661,7 @@
       </c>
       <c r="B49" s="6">
         <f ca="1">Sheet1!K67</f>
-        <v>119</v>
+        <v>119.75</v>
       </c>
     </row>
     <row r="50" spans="1:2">
@@ -3544,7 +3670,7 @@
       </c>
       <c r="B50" s="6">
         <f ca="1">Sheet1!K68</f>
-        <v>114</v>
+        <v>114.3</v>
       </c>
     </row>
     <row r="51" spans="1:2">
@@ -3553,7 +3679,7 @@
       </c>
       <c r="B51" s="6">
         <f ca="1">Sheet1!K69</f>
-        <v>112</v>
+        <v>112.51</v>
       </c>
     </row>
   </sheetData>
@@ -3628,7 +3754,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" cm="1">
@@ -3682,11 +3808,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4EFD4523-7F16-4EE5-BC77-7F896A2520B8}">
   <dimension ref="A1:X90"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" workbookViewId="0">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="K20" sqref="K20:K69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <sheetData>
     <row r="1" spans="1:24">
       <c r="I1">
@@ -4916,8 +5042,8 @@
         <v>112</v>
       </c>
       <c r="K20">
-        <f ca="1">J20+F12</f>
-        <v>112</v>
+        <f ca="1">J20+F12+ROUND(D20,2)</f>
+        <v>112.52</v>
       </c>
     </row>
     <row r="21" spans="1:24">
@@ -4951,8 +5077,8 @@
         <v>100</v>
       </c>
       <c r="K21">
-        <f t="shared" ref="K21:K69" ca="1" si="8">J21+F13</f>
-        <v>100</v>
+        <f t="shared" ref="K21:K69" ca="1" si="8">J21+F13+ROUND(D21,2)</f>
+        <v>100.13</v>
       </c>
     </row>
     <row r="22" spans="1:24">
@@ -4987,7 +5113,7 @@
       </c>
       <c r="K22">
         <f t="shared" ca="1" si="8"/>
-        <v>128</v>
+        <v>128.49</v>
       </c>
       <c r="N22" s="41"/>
     </row>
@@ -5023,7 +5149,7 @@
       </c>
       <c r="K23">
         <f t="shared" ca="1" si="8"/>
-        <v>120</v>
+        <v>120.74</v>
       </c>
       <c r="N23" s="41"/>
     </row>
@@ -5059,7 +5185,7 @@
       </c>
       <c r="K24">
         <f t="shared" ca="1" si="8"/>
-        <v>142</v>
+        <v>142.01</v>
       </c>
       <c r="N24" s="41"/>
     </row>
@@ -5095,7 +5221,7 @@
       </c>
       <c r="K25">
         <f t="shared" ca="1" si="8"/>
-        <v>118</v>
+        <v>118.38</v>
       </c>
       <c r="N25" s="41"/>
     </row>
@@ -5131,7 +5257,7 @@
       </c>
       <c r="K26">
         <f t="shared" ca="1" si="8"/>
-        <v>106</v>
+        <v>106.86</v>
       </c>
       <c r="N26" s="41"/>
     </row>
@@ -5167,7 +5293,7 @@
       </c>
       <c r="K27">
         <f t="shared" ca="1" si="8"/>
-        <v>110</v>
+        <v>110.76</v>
       </c>
       <c r="N27" s="41"/>
     </row>
@@ -5203,7 +5329,7 @@
       </c>
       <c r="K28">
         <f t="shared" ca="1" si="8"/>
-        <v>114</v>
+        <v>114.66</v>
       </c>
       <c r="N28" s="41"/>
     </row>
@@ -5239,7 +5365,7 @@
       </c>
       <c r="K29">
         <f t="shared" ca="1" si="8"/>
-        <v>112</v>
+        <v>112.59</v>
       </c>
       <c r="N29" s="41"/>
     </row>
@@ -5275,7 +5401,7 @@
       </c>
       <c r="K30">
         <f t="shared" ca="1" si="8"/>
-        <v>95</v>
+        <v>95.62</v>
       </c>
       <c r="N30" s="41"/>
     </row>
@@ -5311,7 +5437,7 @@
       </c>
       <c r="K31">
         <f t="shared" ca="1" si="8"/>
-        <v>125</v>
+        <v>125.29</v>
       </c>
       <c r="N31" s="41"/>
     </row>
@@ -5347,7 +5473,7 @@
       </c>
       <c r="K32">
         <f t="shared" ca="1" si="8"/>
-        <v>117</v>
+        <v>117.3</v>
       </c>
       <c r="N32" s="41"/>
     </row>
@@ -5383,7 +5509,7 @@
       </c>
       <c r="K33">
         <f t="shared" ca="1" si="8"/>
-        <v>112</v>
+        <v>112.74</v>
       </c>
       <c r="N33" s="41"/>
     </row>
@@ -5419,7 +5545,7 @@
       </c>
       <c r="K34">
         <f t="shared" ca="1" si="8"/>
-        <v>118</v>
+        <v>118.35</v>
       </c>
     </row>
     <row r="35" spans="1:14">
@@ -5454,7 +5580,7 @@
       </c>
       <c r="K35">
         <f t="shared" ca="1" si="8"/>
-        <v>121</v>
+        <v>121.05</v>
       </c>
     </row>
     <row r="36" spans="1:14">
@@ -5489,7 +5615,7 @@
       </c>
       <c r="K36">
         <f t="shared" ca="1" si="8"/>
-        <v>114</v>
+        <v>114.27</v>
       </c>
     </row>
     <row r="37" spans="1:14">
@@ -5524,7 +5650,7 @@
       </c>
       <c r="K37">
         <f t="shared" ca="1" si="8"/>
-        <v>114</v>
+        <v>114.29</v>
       </c>
     </row>
     <row r="38" spans="1:14">
@@ -5559,7 +5685,7 @@
       </c>
       <c r="K38">
         <f t="shared" ca="1" si="8"/>
-        <v>111</v>
+        <v>111.14</v>
       </c>
     </row>
     <row r="39" spans="1:14">
@@ -5594,7 +5720,7 @@
       </c>
       <c r="K39">
         <f t="shared" ca="1" si="8"/>
-        <v>109</v>
+        <v>109.26</v>
       </c>
     </row>
     <row r="40" spans="1:14">
@@ -5629,7 +5755,7 @@
       </c>
       <c r="K40">
         <f t="shared" ca="1" si="8"/>
-        <v>104</v>
+        <v>104.41</v>
       </c>
     </row>
     <row r="41" spans="1:14">
@@ -5664,7 +5790,7 @@
       </c>
       <c r="K41">
         <f t="shared" ca="1" si="8"/>
-        <v>119</v>
+        <v>119.21</v>
       </c>
     </row>
     <row r="42" spans="1:14">
@@ -5699,7 +5825,7 @@
       </c>
       <c r="K42">
         <f t="shared" ca="1" si="8"/>
-        <v>114</v>
+        <v>114.6</v>
       </c>
     </row>
     <row r="43" spans="1:14">
@@ -5734,7 +5860,7 @@
       </c>
       <c r="K43">
         <f t="shared" ca="1" si="8"/>
-        <v>115</v>
+        <v>115.64</v>
       </c>
     </row>
     <row r="44" spans="1:14">
@@ -5769,7 +5895,7 @@
       </c>
       <c r="K44">
         <f t="shared" ca="1" si="8"/>
-        <v>118</v>
+        <v>118.08</v>
       </c>
     </row>
     <row r="45" spans="1:14">
@@ -5804,7 +5930,7 @@
       </c>
       <c r="K45">
         <f t="shared" ca="1" si="8"/>
-        <v>117</v>
+        <v>117.98</v>
       </c>
     </row>
     <row r="46" spans="1:14">
@@ -5839,7 +5965,7 @@
       </c>
       <c r="K46">
         <f t="shared" ca="1" si="8"/>
-        <v>118</v>
+        <v>118.82</v>
       </c>
     </row>
     <row r="47" spans="1:14">
@@ -5874,7 +6000,7 @@
       </c>
       <c r="K47">
         <f t="shared" ca="1" si="8"/>
-        <v>125</v>
+        <v>125.41</v>
       </c>
     </row>
     <row r="48" spans="1:14">
@@ -5909,7 +6035,7 @@
       </c>
       <c r="K48">
         <f t="shared" ca="1" si="8"/>
-        <v>106</v>
+        <v>106.12</v>
       </c>
     </row>
     <row r="49" spans="1:11">
@@ -5944,7 +6070,7 @@
       </c>
       <c r="K49">
         <f t="shared" ca="1" si="8"/>
-        <v>108</v>
+        <v>108.56</v>
       </c>
     </row>
     <row r="50" spans="1:11">
@@ -5979,7 +6105,7 @@
       </c>
       <c r="K50">
         <f t="shared" ca="1" si="8"/>
-        <v>122</v>
+        <v>122.38</v>
       </c>
     </row>
     <row r="51" spans="1:11">
@@ -6014,7 +6140,7 @@
       </c>
       <c r="K51">
         <f t="shared" ca="1" si="8"/>
-        <v>114</v>
+        <v>114.29</v>
       </c>
     </row>
     <row r="52" spans="1:11">
@@ -6049,7 +6175,7 @@
       </c>
       <c r="K52">
         <f t="shared" ca="1" si="8"/>
-        <v>109</v>
+        <v>109.86</v>
       </c>
     </row>
     <row r="53" spans="1:11">
@@ -6084,7 +6210,7 @@
       </c>
       <c r="K53">
         <f t="shared" ca="1" si="8"/>
-        <v>121</v>
+        <v>121.42</v>
       </c>
     </row>
     <row r="54" spans="1:11">
@@ -6119,7 +6245,7 @@
       </c>
       <c r="K54">
         <f t="shared" ca="1" si="8"/>
-        <v>121</v>
+        <v>121.39</v>
       </c>
     </row>
     <row r="55" spans="1:11">
@@ -6154,7 +6280,7 @@
       </c>
       <c r="K55">
         <f t="shared" ca="1" si="8"/>
-        <v>120</v>
+        <v>120.49</v>
       </c>
     </row>
     <row r="56" spans="1:11">
@@ -6189,7 +6315,7 @@
       </c>
       <c r="K56">
         <f t="shared" ca="1" si="8"/>
-        <v>118</v>
+        <v>118.16</v>
       </c>
     </row>
     <row r="57" spans="1:11">
@@ -6224,7 +6350,7 @@
       </c>
       <c r="K57">
         <f t="shared" ca="1" si="8"/>
-        <v>117</v>
+        <v>117.52</v>
       </c>
     </row>
     <row r="58" spans="1:11">
@@ -6259,7 +6385,7 @@
       </c>
       <c r="K58">
         <f t="shared" ca="1" si="8"/>
-        <v>104</v>
+        <v>104.44</v>
       </c>
     </row>
     <row r="59" spans="1:11">
@@ -6294,7 +6420,7 @@
       </c>
       <c r="K59">
         <f t="shared" ca="1" si="8"/>
-        <v>110</v>
+        <v>110.74</v>
       </c>
     </row>
     <row r="60" spans="1:11">
@@ -6329,7 +6455,7 @@
       </c>
       <c r="K60">
         <f t="shared" ca="1" si="8"/>
-        <v>129</v>
+        <v>129.35</v>
       </c>
     </row>
     <row r="61" spans="1:11">
@@ -6364,7 +6490,7 @@
       </c>
       <c r="K61">
         <f t="shared" ca="1" si="8"/>
-        <v>113</v>
+        <v>113.34</v>
       </c>
     </row>
     <row r="62" spans="1:11">
@@ -6399,7 +6525,7 @@
       </c>
       <c r="K62">
         <f t="shared" ca="1" si="8"/>
-        <v>120</v>
+        <v>120.61</v>
       </c>
     </row>
     <row r="63" spans="1:11">
@@ -6434,7 +6560,7 @@
       </c>
       <c r="K63">
         <f t="shared" ca="1" si="8"/>
-        <v>117</v>
+        <v>117.25</v>
       </c>
     </row>
     <row r="64" spans="1:11">
@@ -6469,7 +6595,7 @@
       </c>
       <c r="K64">
         <f t="shared" ca="1" si="8"/>
-        <v>103</v>
+        <v>103.28</v>
       </c>
     </row>
     <row r="65" spans="1:11">
@@ -6504,7 +6630,7 @@
       </c>
       <c r="K65">
         <f t="shared" ca="1" si="8"/>
-        <v>115</v>
+        <v>115.85</v>
       </c>
     </row>
     <row r="66" spans="1:11">
@@ -6539,7 +6665,7 @@
       </c>
       <c r="K66">
         <f t="shared" ca="1" si="8"/>
-        <v>114</v>
+        <v>114.51</v>
       </c>
     </row>
     <row r="67" spans="1:11">
@@ -6574,7 +6700,7 @@
       </c>
       <c r="K67">
         <f t="shared" ca="1" si="8"/>
-        <v>119</v>
+        <v>119.75</v>
       </c>
     </row>
     <row r="68" spans="1:11">
@@ -6609,7 +6735,7 @@
       </c>
       <c r="K68">
         <f t="shared" ca="1" si="8"/>
-        <v>114</v>
+        <v>114.3</v>
       </c>
     </row>
     <row r="69" spans="1:11">
@@ -6644,7 +6770,7 @@
       </c>
       <c r="K69">
         <f t="shared" ca="1" si="8"/>
-        <v>112</v>
+        <v>112.51</v>
       </c>
     </row>
     <row r="70" spans="1:11">
@@ -7179,21 +7305,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7437,19 +7563,19 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73BD24FA-A4D4-4F71-A18A-C8260E97BFC1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23FC55F1-8C15-4A13-B875-E9240B3D0196}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{23FC55F1-8C15-4A13-B875-E9240B3D0196}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{73BD24FA-A4D4-4F71-A18A-C8260E97BFC1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>